<commit_message>
checking git diff for excel
</commit_message>
<xml_diff>
--- a/collections.xlsx
+++ b/collections.xlsx
@@ -4713,10 +4713,10 @@
   <dimension ref="A1:P418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B241" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P223" sqref="P223"/>
+      <selection pane="bottomRight" activeCell="L262" sqref="L262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16253,6 +16253,15 @@
       <c r="D261" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J261" s="9">
+        <v>38.223466999999999</v>
+      </c>
+      <c r="K261" s="9">
+        <v>119.99784699999999</v>
+      </c>
+      <c r="L261" s="1">
+        <v>5838</v>
+      </c>
     </row>
     <row r="262" spans="1:16">
       <c r="A262" s="17">

</xml_diff>